<commit_message>
[Item Suffixes] Life regen bonuses; modified the blacklist and item name handling a little
</commit_message>
<xml_diff>
--- a/Item Suffixes/Spreadsheet.xlsx
+++ b/Item Suffixes/Spreadsheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="28695" windowHeight="12270"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
   <si>
     <t>Bear</t>
   </si>
@@ -118,13 +118,43 @@
   </si>
   <si>
     <t>++</t>
+  </si>
+  <si>
+    <t>HP regen</t>
+  </si>
+  <si>
+    <t>Regeneration</t>
+  </si>
+  <si>
+    <t>Boar</t>
+  </si>
+  <si>
+    <t>Bandit</t>
+  </si>
+  <si>
+    <t>Marksmanship</t>
+  </si>
+  <si>
+    <t>Eluding</t>
+  </si>
+  <si>
+    <t>Necromancer</t>
+  </si>
+  <si>
+    <t>Concentration</t>
+  </si>
+  <si>
+    <t>Paladin</t>
+  </si>
+  <si>
+    <t>Elder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -390,11 +420,124 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -445,11 +588,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="2">
     <dxf>
       <font>
         <condense val="0"/>
@@ -474,51 +645,13 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -597,6 +730,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -631,6 +765,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -806,20 +941,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="9" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="10" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="78.75" thickTop="1" thickBot="1">
+    <row r="1" spans="1:10" ht="78.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="17" t="s">
         <v>24</v>
@@ -842,11 +977,14 @@
       <c r="H1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="24" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickTop="1">
+      <c r="J1" s="19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -861,9 +999,10 @@
       <c r="H2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="I2" s="25"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
@@ -876,11 +1015,12 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="I3" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
@@ -895,9 +1035,10 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="I4" s="26"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
@@ -910,9 +1051,10 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="I5" s="26"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>4</v>
       </c>
@@ -925,9 +1067,10 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="I6" s="26"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>5</v>
       </c>
@@ -942,9 +1085,10 @@
       <c r="H7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="I7" s="26"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>6</v>
       </c>
@@ -957,11 +1101,12 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="I8" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>7</v>
       </c>
@@ -976,9 +1121,10 @@
       <c r="H9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="I9" s="26"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
@@ -991,11 +1137,12 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="I10" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>9</v>
       </c>
@@ -1010,9 +1157,10 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="I11" s="26"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>10</v>
       </c>
@@ -1025,9 +1173,10 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="I12" s="26"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>11</v>
       </c>
@@ -1040,9 +1189,10 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="I13" s="26"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>12</v>
       </c>
@@ -1057,9 +1207,10 @@
       <c r="H14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="I14" s="26"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>13</v>
       </c>
@@ -1072,11 +1223,12 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="I15" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>14</v>
       </c>
@@ -1091,9 +1243,10 @@
       <c r="H16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="I16" s="26"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>15</v>
       </c>
@@ -1106,11 +1259,12 @@
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="I17" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>16</v>
       </c>
@@ -1125,9 +1279,10 @@
         <v>32</v>
       </c>
       <c r="H18" s="6"/>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="I18" s="26"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>17</v>
       </c>
@@ -1140,9 +1295,10 @@
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
-      <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="I19" s="26"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>18</v>
       </c>
@@ -1155,9 +1311,10 @@
         <v>33</v>
       </c>
       <c r="H20" s="6"/>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="I20" s="26"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>19</v>
       </c>
@@ -1172,9 +1329,10 @@
       <c r="H21" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="I21" s="26"/>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>20</v>
       </c>
@@ -1187,11 +1345,12 @@
         <v>32</v>
       </c>
       <c r="H22" s="6"/>
-      <c r="I22" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="I22" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>21</v>
       </c>
@@ -1204,9 +1363,10 @@
       <c r="H23" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="I23" s="27"/>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>22</v>
       </c>
@@ -1217,35 +1377,197 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
-      <c r="I24" s="10" t="s">
+      <c r="I24" s="27" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A25" s="16" t="s">
+      <c r="J24" s="10"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="I25" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" thickTop="1"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="J25" s="23"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="21"/>
+      <c r="C28" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="21"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H32" s="22"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="21"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I33" s="28"/>
+      <c r="J33" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="11"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="B2:I25">
+  <conditionalFormatting sqref="B2:J34">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"++"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"+"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"++"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1257,24 +1579,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>